<commit_message>
Added BDDAD additional data for sprint 3. Feat: calculus for area in ha, when adding permanent plantations. BugFix: fixed minor bugs on importing data for products. New inserts file for sprint 3.
</commit_message>
<xml_diff>
--- a/files/Legacy_Data_v2a.xlsx
+++ b/files/Legacy_Data_v2a.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcaro\PI3\lapr3-2023-2024-group322\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcaro\PI3\lapr3-2023-2024-group322_main\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24556E40-62AF-494E-BBEE-9BDA94BE8093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C86260-A082-442D-8E6C-416F3AD97DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{ACBD79A1-D35B-4D3E-A78E-4F35CA726952}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{ACBD79A1-D35B-4D3E-A78E-4F35CA726952}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantas" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Operações!$A$1:$I$209</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plantas!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1748" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="256">
   <si>
     <t>Espécie</t>
   </si>
@@ -720,9 +721,6 @@
     <t>S. Cosme</t>
   </si>
   <si>
-    <t>Fevereiro a abril, agosto a outubro</t>
-  </si>
-  <si>
     <t>90 dias</t>
   </si>
   <si>
@@ -811,6 +809,9 @@
   </si>
   <si>
     <t>Galega</t>
+  </si>
+  <si>
+    <t>Fevereiro a abril</t>
   </si>
 </sst>
 </file>
@@ -1189,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA74F46-7FB7-481B-9DAE-CE325D568C4A}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,9 +1200,9 @@
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" customWidth="1"/>
   </cols>
@@ -3186,7 +3187,7 @@
         <v>124</v>
       </c>
       <c r="C93" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D93" t="s">
         <v>11</v>
@@ -3209,59 +3210,60 @@
         <v>99</v>
       </c>
       <c r="E94" t="s">
+        <v>255</v>
+      </c>
+      <c r="H94" t="s">
         <v>225</v>
-      </c>
-      <c r="H94" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>239</v>
+      </c>
+      <c r="B95" t="s">
         <v>240</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>241</v>
-      </c>
-      <c r="C95" t="s">
-        <v>242</v>
       </c>
       <c r="D95" t="s">
         <v>11</v>
       </c>
       <c r="F95" t="s">
+        <v>243</v>
+      </c>
+      <c r="G95" t="s">
+        <v>242</v>
+      </c>
+      <c r="H95" t="s">
         <v>244</v>
-      </c>
-      <c r="G95" t="s">
-        <v>243</v>
-      </c>
-      <c r="H95" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>239</v>
+      </c>
+      <c r="B96" t="s">
         <v>240</v>
       </c>
-      <c r="B96" t="s">
-        <v>241</v>
-      </c>
       <c r="C96" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D96" t="s">
         <v>11</v>
       </c>
       <c r="F96" t="s">
+        <v>243</v>
+      </c>
+      <c r="G96" t="s">
+        <v>242</v>
+      </c>
+      <c r="H96" t="s">
         <v>244</v>
       </c>
-      <c r="G96" t="s">
-        <v>243</v>
-      </c>
-      <c r="H96" t="s">
-        <v>245</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{5CA74F46-7FB7-481B-9DAE-CE325D568C4A}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3578,13 +3580,13 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B10" t="s">
         <v>150</v>
       </c>
       <c r="C10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D10" t="s">
         <v>146</v>
@@ -3593,7 +3595,7 @@
         <v>147</v>
       </c>
       <c r="F10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G10" s="4">
         <v>0.97740000000000005</v>
@@ -3601,22 +3603,22 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B11" t="s">
         <v>150</v>
       </c>
       <c r="C11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D11" t="s">
         <v>146</v>
       </c>
       <c r="E11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G11" s="4">
         <v>0.47799999999999998</v>
@@ -3624,22 +3626,22 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B12" t="s">
         <v>150</v>
       </c>
       <c r="C12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D12" t="s">
         <v>146</v>
       </c>
       <c r="E12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G12" s="4">
         <v>0.14419999999999999</v>
@@ -3676,7 +3678,7 @@
         <v>133</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>176</v>
@@ -3792,7 +3794,7 @@
         <v>177</v>
       </c>
       <c r="C8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -3888,7 +3890,7 @@
         <v>191</v>
       </c>
       <c r="C14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D14">
         <v>35</v>
@@ -3910,8 +3912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246DE277-EC3F-46EA-8D39-A978B7AEA5AE}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4060,7 +4062,7 @@
         <v>181</v>
       </c>
       <c r="C6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D6" t="s">
         <v>99</v>
@@ -4112,7 +4114,7 @@
         <v>181</v>
       </c>
       <c r="C8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D8" t="s">
         <v>99</v>
@@ -4164,7 +4166,7 @@
         <v>181</v>
       </c>
       <c r="C10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D10" t="s">
         <v>99</v>
@@ -4314,7 +4316,7 @@
         <v>220</v>
       </c>
       <c r="C16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D16" t="s">
         <v>99</v>
@@ -4340,7 +4342,7 @@
         <v>220</v>
       </c>
       <c r="C17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D17" t="s">
         <v>99</v>
@@ -4366,7 +4368,7 @@
         <v>220</v>
       </c>
       <c r="C18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D18" t="s">
         <v>99</v>
@@ -4392,7 +4394,7 @@
         <v>220</v>
       </c>
       <c r="C19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D19" t="s">
         <v>99</v>
@@ -4418,7 +4420,7 @@
         <v>220</v>
       </c>
       <c r="C20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D20" t="s">
         <v>99</v>
@@ -4470,7 +4472,7 @@
         <v>220</v>
       </c>
       <c r="C22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D22" t="s">
         <v>99</v>
@@ -4585,10 +4587,10 @@
         <v>107</v>
       </c>
       <c r="B27" t="s">
+        <v>245</v>
+      </c>
+      <c r="C27" t="s">
         <v>246</v>
-      </c>
-      <c r="C27" t="s">
-        <v>247</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -4608,10 +4610,10 @@
         <v>107</v>
       </c>
       <c r="B28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C28" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -4638,11 +4640,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8273E431-88A0-4D26-AA21-9E0D94FE2923}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E159" sqref="E159"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H135" sqref="H135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4686,7 +4687,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>102</v>
       </c>
@@ -4709,7 +4710,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>102</v>
       </c>
@@ -4732,7 +4733,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>104</v>
       </c>
@@ -4755,7 +4756,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>104</v>
       </c>
@@ -4778,7 +4779,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>104</v>
       </c>
@@ -4801,7 +4802,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>102</v>
       </c>
@@ -4824,7 +4825,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>102</v>
       </c>
@@ -4847,7 +4848,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>104</v>
       </c>
@@ -4870,7 +4871,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>102</v>
       </c>
@@ -4893,7 +4894,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>102</v>
       </c>
@@ -4916,7 +4917,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>104</v>
       </c>
@@ -4939,7 +4940,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>104</v>
       </c>
@@ -4962,7 +4963,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>102</v>
       </c>
@@ -4985,7 +4986,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>102</v>
       </c>
@@ -5008,7 +5009,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>102</v>
       </c>
@@ -5019,7 +5020,7 @@
         <v>216</v>
       </c>
       <c r="D16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E16" t="s">
         <v>200</v>
@@ -5037,7 +5038,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>102</v>
       </c>
@@ -5048,7 +5049,7 @@
         <v>216</v>
       </c>
       <c r="D17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E17" t="s">
         <v>202</v>
@@ -5066,7 +5067,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>104</v>
       </c>
@@ -5089,7 +5090,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>104</v>
       </c>
@@ -5112,7 +5113,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>104</v>
       </c>
@@ -5135,18 +5136,18 @@
         <v>201</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>107</v>
       </c>
       <c r="B21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C21" t="s">
         <v>213</v>
       </c>
       <c r="E21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F21" s="1">
         <v>43110</v>
@@ -5158,18 +5159,18 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>107</v>
       </c>
       <c r="B22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C22" t="s">
         <v>213</v>
       </c>
       <c r="E22" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F22" s="1">
         <v>43111</v>
@@ -5181,7 +5182,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>104</v>
       </c>
@@ -5192,7 +5193,7 @@
         <v>216</v>
       </c>
       <c r="D23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E23" t="s">
         <v>203</v>
@@ -5210,7 +5211,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>104</v>
       </c>
@@ -5221,7 +5222,7 @@
         <v>216</v>
       </c>
       <c r="D24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E24" t="s">
         <v>204</v>
@@ -5239,7 +5240,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>104</v>
       </c>
@@ -5250,7 +5251,7 @@
         <v>216</v>
       </c>
       <c r="D25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E25" t="s">
         <v>205</v>
@@ -5268,7 +5269,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>102</v>
       </c>
@@ -5291,7 +5292,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>102</v>
       </c>
@@ -5314,7 +5315,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>104</v>
       </c>
@@ -5337,18 +5338,18 @@
         <v>193</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>107</v>
       </c>
       <c r="B29" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C29" t="s">
         <v>191</v>
       </c>
       <c r="E29" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F29" s="1">
         <v>43291</v>
@@ -5360,7 +5361,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>102</v>
       </c>
@@ -5383,7 +5384,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>102</v>
       </c>
@@ -5406,7 +5407,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>104</v>
       </c>
@@ -5429,18 +5430,18 @@
         <v>193</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>107</v>
       </c>
       <c r="B33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C33" t="s">
         <v>191</v>
       </c>
       <c r="E33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F33" s="1">
         <v>43323</v>
@@ -5452,7 +5453,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>104</v>
       </c>
@@ -5475,7 +5476,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>104</v>
       </c>
@@ -5498,7 +5499,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>102</v>
       </c>
@@ -5521,7 +5522,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>102</v>
       </c>
@@ -5544,7 +5545,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>104</v>
       </c>
@@ -5567,18 +5568,18 @@
         <v>201</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>107</v>
       </c>
       <c r="B39" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F39" s="1">
         <v>43450</v>
@@ -5590,18 +5591,18 @@
         <v>201</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>107</v>
       </c>
       <c r="B40" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F40" s="1">
         <v>43452</v>
@@ -5613,7 +5614,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>104</v>
       </c>
@@ -5636,7 +5637,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>104</v>
       </c>
@@ -5659,7 +5660,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>104</v>
       </c>
@@ -5682,18 +5683,18 @@
         <v>201</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>107</v>
       </c>
       <c r="B44" t="s">
+        <v>245</v>
+      </c>
+      <c r="C44" t="s">
+        <v>251</v>
+      </c>
+      <c r="E44" t="s">
         <v>246</v>
-      </c>
-      <c r="C44" t="s">
-        <v>252</v>
-      </c>
-      <c r="E44" t="s">
-        <v>247</v>
       </c>
       <c r="F44" s="1">
         <v>43485</v>
@@ -5708,18 +5709,18 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>107</v>
       </c>
       <c r="B45" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C45" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E45" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F45" s="1">
         <v>43485</v>
@@ -5734,7 +5735,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>104</v>
       </c>
@@ -5745,7 +5746,7 @@
         <v>216</v>
       </c>
       <c r="D46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E46" t="s">
         <v>203</v>
@@ -5763,7 +5764,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>104</v>
       </c>
@@ -5774,7 +5775,7 @@
         <v>216</v>
       </c>
       <c r="D47" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E47" t="s">
         <v>204</v>
@@ -5792,7 +5793,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>104</v>
       </c>
@@ -5803,7 +5804,7 @@
         <v>216</v>
       </c>
       <c r="D48" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E48" t="s">
         <v>205</v>
@@ -5821,7 +5822,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>102</v>
       </c>
@@ -5844,7 +5845,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>102</v>
       </c>
@@ -5867,7 +5868,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>104</v>
       </c>
@@ -5890,18 +5891,18 @@
         <v>193</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>107</v>
       </c>
       <c r="B52" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C52" t="s">
         <v>191</v>
       </c>
       <c r="E52" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F52" s="1">
         <v>43656</v>
@@ -5913,7 +5914,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>102</v>
       </c>
@@ -5936,7 +5937,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>102</v>
       </c>
@@ -5959,7 +5960,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>104</v>
       </c>
@@ -5982,18 +5983,18 @@
         <v>193</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>107</v>
       </c>
       <c r="B56" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C56" t="s">
         <v>191</v>
       </c>
       <c r="E56" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F56" s="1">
         <v>43688</v>
@@ -6005,7 +6006,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>102</v>
       </c>
@@ -6028,7 +6029,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>102</v>
       </c>
@@ -6051,18 +6052,18 @@
         <v>201</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>107</v>
       </c>
       <c r="B59" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
       </c>
       <c r="E59" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F59" s="1">
         <v>43815</v>
@@ -6074,18 +6075,18 @@
         <v>201</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>107</v>
       </c>
       <c r="B60" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
       </c>
       <c r="E60" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F60" s="1">
         <v>43817</v>
@@ -6097,18 +6098,18 @@
         <v>201</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>107</v>
       </c>
       <c r="B61" t="s">
+        <v>245</v>
+      </c>
+      <c r="C61" t="s">
+        <v>251</v>
+      </c>
+      <c r="E61" t="s">
         <v>246</v>
-      </c>
-      <c r="C61" t="s">
-        <v>252</v>
-      </c>
-      <c r="E61" t="s">
-        <v>247</v>
       </c>
       <c r="F61" s="1">
         <v>43850</v>
@@ -6123,18 +6124,18 @@
         <v>143</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>107</v>
       </c>
       <c r="B62" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C62" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E62" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F62" s="1">
         <v>43850</v>
@@ -6149,7 +6150,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>106</v>
       </c>
@@ -6172,7 +6173,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>103</v>
       </c>
@@ -6183,7 +6184,7 @@
         <v>216</v>
       </c>
       <c r="D64" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F64" s="1">
         <v>43920</v>
@@ -6198,7 +6199,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>103</v>
       </c>
@@ -6209,7 +6210,7 @@
         <v>214</v>
       </c>
       <c r="E65" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F65" s="1">
         <v>43926</v>
@@ -6221,7 +6222,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>106</v>
       </c>
@@ -6244,7 +6245,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>106</v>
       </c>
@@ -6267,7 +6268,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>106</v>
       </c>
@@ -6290,7 +6291,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>102</v>
       </c>
@@ -6313,7 +6314,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>102</v>
       </c>
@@ -6336,18 +6337,18 @@
         <v>193</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>107</v>
       </c>
       <c r="B71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C71" t="s">
         <v>191</v>
       </c>
       <c r="E71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F71" s="1">
         <v>44022</v>
@@ -6359,7 +6360,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>103</v>
       </c>
@@ -6370,7 +6371,7 @@
         <v>191</v>
       </c>
       <c r="E72" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F72" s="1">
         <v>44024</v>
@@ -6382,7 +6383,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>106</v>
       </c>
@@ -6405,7 +6406,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>103</v>
       </c>
@@ -6416,7 +6417,7 @@
         <v>191</v>
       </c>
       <c r="E74" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F74" s="1">
         <v>44040</v>
@@ -6428,7 +6429,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>102</v>
       </c>
@@ -6451,7 +6452,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>102</v>
       </c>
@@ -6474,7 +6475,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>103</v>
       </c>
@@ -6485,7 +6486,7 @@
         <v>191</v>
       </c>
       <c r="E77" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F77" s="1">
         <v>44053</v>
@@ -6497,18 +6498,18 @@
         <v>193</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>107</v>
       </c>
       <c r="B78" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C78" t="s">
         <v>191</v>
       </c>
       <c r="E78" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F78" s="1">
         <v>44054</v>
@@ -6520,7 +6521,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>106</v>
       </c>
@@ -6543,7 +6544,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>103</v>
       </c>
@@ -6554,7 +6555,7 @@
         <v>7</v>
       </c>
       <c r="E80" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F80" s="1">
         <v>44063</v>
@@ -6566,7 +6567,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>106</v>
       </c>
@@ -6589,7 +6590,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>106</v>
       </c>
@@ -6612,7 +6613,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>106</v>
       </c>
@@ -6623,7 +6624,7 @@
         <v>214</v>
       </c>
       <c r="E83" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F83" s="1">
         <v>44094</v>
@@ -6635,7 +6636,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>101</v>
       </c>
@@ -6658,7 +6659,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>103</v>
       </c>
@@ -6681,7 +6682,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>102</v>
       </c>
@@ -6704,7 +6705,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>102</v>
       </c>
@@ -6727,7 +6728,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>106</v>
       </c>
@@ -6738,7 +6739,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F88" s="1">
         <v>44150</v>
@@ -6796,7 +6797,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>102</v>
       </c>
@@ -6807,7 +6808,7 @@
         <v>216</v>
       </c>
       <c r="D91" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E91" t="s">
         <v>200</v>
@@ -6825,7 +6826,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>102</v>
       </c>
@@ -6836,7 +6837,7 @@
         <v>216</v>
       </c>
       <c r="D92" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E92" t="s">
         <v>202</v>
@@ -6900,18 +6901,18 @@
         <v>201</v>
       </c>
     </row>
-    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>107</v>
       </c>
       <c r="B95" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C95" t="s">
         <v>5</v>
       </c>
       <c r="E95" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F95" s="1">
         <v>44181</v>
@@ -6923,7 +6924,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>106</v>
       </c>
@@ -6934,7 +6935,7 @@
         <v>7</v>
       </c>
       <c r="E96" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F96" s="1">
         <v>44183</v>
@@ -6946,18 +6947,18 @@
         <v>218</v>
       </c>
     </row>
-    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>107</v>
       </c>
       <c r="B97" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C97" t="s">
         <v>5</v>
       </c>
       <c r="E97" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F97" s="1">
         <v>44183</v>
@@ -6969,7 +6970,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>106</v>
       </c>
@@ -6980,7 +6981,7 @@
         <v>7</v>
       </c>
       <c r="E98" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F98" s="1">
         <v>44200</v>
@@ -6992,18 +6993,18 @@
         <v>218</v>
       </c>
     </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>107</v>
       </c>
       <c r="B99" t="s">
+        <v>245</v>
+      </c>
+      <c r="C99" t="s">
+        <v>251</v>
+      </c>
+      <c r="E99" t="s">
         <v>246</v>
-      </c>
-      <c r="C99" t="s">
-        <v>252</v>
-      </c>
-      <c r="E99" t="s">
-        <v>247</v>
       </c>
       <c r="F99" s="1">
         <v>44216</v>
@@ -7018,18 +7019,18 @@
         <v>143</v>
       </c>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>107</v>
       </c>
       <c r="B100" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C100" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E100" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F100" s="1">
         <v>44216</v>
@@ -7044,7 +7045,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>106</v>
       </c>
@@ -7055,7 +7056,7 @@
         <v>214</v>
       </c>
       <c r="E101" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F101" s="1">
         <v>44265</v>
@@ -7067,7 +7068,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>103</v>
       </c>
@@ -7090,7 +7091,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>101</v>
       </c>
@@ -7113,7 +7114,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -7124,7 +7125,7 @@
         <v>214</v>
       </c>
       <c r="E104" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F104" s="1">
         <v>44289</v>
@@ -7136,7 +7137,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>101</v>
       </c>
@@ -7188,7 +7189,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -7199,7 +7200,7 @@
         <v>7</v>
       </c>
       <c r="E107" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F107" s="1">
         <v>44321</v>
@@ -7211,7 +7212,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>106</v>
       </c>
@@ -7222,7 +7223,7 @@
         <v>7</v>
       </c>
       <c r="E108" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F108" s="1">
         <v>44331</v>
@@ -7234,7 +7235,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>106</v>
       </c>
@@ -7245,7 +7246,7 @@
         <v>214</v>
       </c>
       <c r="E109" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F109" s="1">
         <v>44349</v>
@@ -7257,7 +7258,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>106</v>
       </c>
@@ -7268,7 +7269,7 @@
         <v>191</v>
       </c>
       <c r="E110" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F110" s="1">
         <v>44367</v>
@@ -7280,7 +7281,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>102</v>
       </c>
@@ -7303,7 +7304,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>102</v>
       </c>
@@ -7349,7 +7350,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>106</v>
       </c>
@@ -7360,7 +7361,7 @@
         <v>191</v>
       </c>
       <c r="E114" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F114" s="1">
         <v>44384</v>
@@ -7372,18 +7373,18 @@
         <v>193</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>107</v>
       </c>
       <c r="B115" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C115" t="s">
         <v>191</v>
       </c>
       <c r="E115" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F115" s="1">
         <v>44387</v>
@@ -7395,7 +7396,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>103</v>
       </c>
@@ -7406,7 +7407,7 @@
         <v>191</v>
       </c>
       <c r="E116" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F116" s="1">
         <v>44389</v>
@@ -7418,18 +7419,18 @@
         <v>193</v>
       </c>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>107</v>
       </c>
       <c r="B117" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C117" t="s">
         <v>7</v>
       </c>
       <c r="E117" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F117" s="1">
         <v>44392</v>
@@ -7441,18 +7442,18 @@
         <v>218</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>107</v>
       </c>
       <c r="B118" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C118" t="s">
         <v>7</v>
       </c>
       <c r="E118" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F118" s="1">
         <v>44397</v>
@@ -7464,7 +7465,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>103</v>
       </c>
@@ -7475,7 +7476,7 @@
         <v>191</v>
       </c>
       <c r="E119" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F119" s="1">
         <v>44401</v>
@@ -7510,7 +7511,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>106</v>
       </c>
@@ -7521,7 +7522,7 @@
         <v>191</v>
       </c>
       <c r="E121" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F121" s="1">
         <v>44407</v>
@@ -7533,7 +7534,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>103</v>
       </c>
@@ -7544,7 +7545,7 @@
         <v>191</v>
       </c>
       <c r="E122" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F122" s="1">
         <v>44415</v>
@@ -7556,7 +7557,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>102</v>
       </c>
@@ -7579,7 +7580,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>102</v>
       </c>
@@ -7602,7 +7603,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>101</v>
       </c>
@@ -7625,7 +7626,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>106</v>
       </c>
@@ -7636,7 +7637,7 @@
         <v>191</v>
       </c>
       <c r="E126" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F126" s="1">
         <v>44425</v>
@@ -7671,7 +7672,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>103</v>
       </c>
@@ -7682,7 +7683,7 @@
         <v>7</v>
       </c>
       <c r="E128" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F128" s="1">
         <v>44433</v>
@@ -7694,7 +7695,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>106</v>
       </c>
@@ -7705,7 +7706,7 @@
         <v>7</v>
       </c>
       <c r="E129" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F129" s="1">
         <v>44436</v>
@@ -7740,7 +7741,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>106</v>
       </c>
@@ -7751,7 +7752,7 @@
         <v>7</v>
       </c>
       <c r="E131" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F131" s="1">
         <v>44446</v>
@@ -7786,7 +7787,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>106</v>
       </c>
@@ -7797,7 +7798,7 @@
         <v>214</v>
       </c>
       <c r="E133" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F133" s="1">
         <v>44459</v>
@@ -7832,7 +7833,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>101</v>
       </c>
@@ -7851,8 +7852,11 @@
       <c r="G135">
         <v>36</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H135" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>103</v>
       </c>
@@ -7921,7 +7925,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>102</v>
       </c>
@@ -7944,7 +7948,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>102</v>
       </c>
@@ -7967,7 +7971,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>106</v>
       </c>
@@ -7978,7 +7982,7 @@
         <v>7</v>
       </c>
       <c r="E141" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F141" s="1">
         <v>44515</v>
@@ -7990,7 +7994,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>102</v>
       </c>
@@ -8013,7 +8017,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>102</v>
       </c>
@@ -8082,18 +8086,18 @@
         <v>201</v>
       </c>
     </row>
-    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>107</v>
       </c>
       <c r="B146" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C146" t="s">
         <v>5</v>
       </c>
       <c r="E146" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F146" s="1">
         <v>44546</v>
@@ -8128,7 +8132,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>106</v>
       </c>
@@ -8139,7 +8143,7 @@
         <v>7</v>
       </c>
       <c r="E148" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F148" s="1">
         <v>44548</v>
@@ -8151,18 +8155,18 @@
         <v>218</v>
       </c>
     </row>
-    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>107</v>
       </c>
       <c r="B149" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C149" t="s">
         <v>5</v>
       </c>
       <c r="E149" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F149" s="1">
         <v>44548</v>
@@ -8174,7 +8178,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>106</v>
       </c>
@@ -8185,7 +8189,7 @@
         <v>7</v>
       </c>
       <c r="E150" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F150" s="1">
         <v>44565</v>
@@ -8197,18 +8201,18 @@
         <v>218</v>
       </c>
     </row>
-    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>107</v>
       </c>
       <c r="B151" t="s">
+        <v>245</v>
+      </c>
+      <c r="C151" t="s">
+        <v>251</v>
+      </c>
+      <c r="E151" t="s">
         <v>246</v>
-      </c>
-      <c r="C151" t="s">
-        <v>252</v>
-      </c>
-      <c r="E151" t="s">
-        <v>247</v>
       </c>
       <c r="F151" s="1">
         <v>44581</v>
@@ -8223,18 +8227,18 @@
         <v>143</v>
       </c>
     </row>
-    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>107</v>
       </c>
       <c r="B152" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C152" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E152" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F152" s="1">
         <v>44581</v>
@@ -8249,7 +8253,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>106</v>
       </c>
@@ -8260,7 +8264,7 @@
         <v>214</v>
       </c>
       <c r="E153" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F153" s="1">
         <v>44626</v>
@@ -8272,7 +8276,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>103</v>
       </c>
@@ -8295,7 +8299,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>101</v>
       </c>
@@ -8318,7 +8322,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>103</v>
       </c>
@@ -8329,7 +8333,7 @@
         <v>214</v>
       </c>
       <c r="E156" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F156" s="1">
         <v>44659</v>
@@ -8341,7 +8345,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>101</v>
       </c>
@@ -8364,7 +8368,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>106</v>
       </c>
@@ -8375,7 +8379,7 @@
         <v>7</v>
       </c>
       <c r="E158" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F158" s="1">
         <v>44686</v>
@@ -8416,7 +8420,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>106</v>
       </c>
@@ -8427,7 +8431,7 @@
         <v>7</v>
       </c>
       <c r="E160" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F160" s="1">
         <v>44696</v>
@@ -8439,7 +8443,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>106</v>
       </c>
@@ -8485,7 +8489,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>106</v>
       </c>
@@ -8531,7 +8535,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>102</v>
       </c>
@@ -8554,7 +8558,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>102</v>
       </c>
@@ -8577,18 +8581,18 @@
         <v>193</v>
       </c>
     </row>
-    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>107</v>
       </c>
       <c r="B167" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C167" t="s">
         <v>191</v>
       </c>
       <c r="E167" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F167" s="1">
         <v>44752</v>
@@ -8600,7 +8604,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>103</v>
       </c>
@@ -8611,7 +8615,7 @@
         <v>191</v>
       </c>
       <c r="E168" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F168" s="1">
         <v>44754</v>
@@ -8623,7 +8627,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>106</v>
       </c>
@@ -8646,18 +8650,18 @@
         <v>193</v>
       </c>
     </row>
-    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>107</v>
       </c>
       <c r="B170" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C170" t="s">
         <v>7</v>
       </c>
       <c r="E170" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F170" s="1">
         <v>44757</v>
@@ -8669,18 +8673,18 @@
         <v>218</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>107</v>
       </c>
       <c r="B171" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C171" t="s">
         <v>7</v>
       </c>
       <c r="E171" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F171" s="1">
         <v>44762</v>
@@ -8692,7 +8696,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>103</v>
       </c>
@@ -8703,7 +8707,7 @@
         <v>191</v>
       </c>
       <c r="E172" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F172" s="1">
         <v>44766</v>
@@ -8738,7 +8742,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>106</v>
       </c>
@@ -8761,7 +8765,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>103</v>
       </c>
@@ -8772,7 +8776,7 @@
         <v>191</v>
       </c>
       <c r="E175" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F175" s="1">
         <v>44780</v>
@@ -8784,7 +8788,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>102</v>
       </c>
@@ -8807,7 +8811,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>102</v>
       </c>
@@ -8830,18 +8834,18 @@
         <v>193</v>
       </c>
     </row>
-    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>107</v>
       </c>
       <c r="B178" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C178" t="s">
         <v>7</v>
       </c>
       <c r="E178" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F178" s="1">
         <v>44785</v>
@@ -8853,18 +8857,18 @@
         <v>218</v>
       </c>
     </row>
-    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>107</v>
       </c>
       <c r="B179" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C179" t="s">
         <v>7</v>
       </c>
       <c r="E179" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F179" s="1">
         <v>44785</v>
@@ -8876,7 +8880,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>101</v>
       </c>
@@ -8899,7 +8903,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>106</v>
       </c>
@@ -8922,7 +8926,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>103</v>
       </c>
@@ -8933,7 +8937,7 @@
         <v>7</v>
       </c>
       <c r="E182" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F182" s="1">
         <v>44791</v>
@@ -8968,7 +8972,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>106</v>
       </c>
@@ -8991,7 +8995,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>106</v>
       </c>
@@ -9083,7 +9087,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>106</v>
       </c>
@@ -9094,7 +9098,7 @@
         <v>214</v>
       </c>
       <c r="E189" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F189" s="1">
         <v>44824</v>
@@ -9106,7 +9110,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>103</v>
       </c>
@@ -9175,7 +9179,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>102</v>
       </c>
@@ -9198,7 +9202,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>102</v>
       </c>
@@ -9221,7 +9225,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>102</v>
       </c>
@@ -9244,7 +9248,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>102</v>
       </c>
@@ -9267,7 +9271,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>106</v>
       </c>
@@ -9278,7 +9282,7 @@
         <v>7</v>
       </c>
       <c r="E197" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F197" s="1">
         <v>44880</v>
@@ -9336,7 +9340,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>102</v>
       </c>
@@ -9347,7 +9351,7 @@
         <v>216</v>
       </c>
       <c r="D200" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E200" t="s">
         <v>200</v>
@@ -9365,7 +9369,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>102</v>
       </c>
@@ -9376,7 +9380,7 @@
         <v>216</v>
       </c>
       <c r="D201" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E201" t="s">
         <v>202</v>
@@ -9394,18 +9398,18 @@
         <v>152</v>
       </c>
     </row>
-    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>107</v>
       </c>
       <c r="B202" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C202" t="s">
         <v>5</v>
       </c>
       <c r="E202" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F202" s="1">
         <v>44911</v>
@@ -9417,7 +9421,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>106</v>
       </c>
@@ -9428,7 +9432,7 @@
         <v>7</v>
       </c>
       <c r="E203" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F203" s="1">
         <v>44913</v>
@@ -9440,18 +9444,18 @@
         <v>218</v>
       </c>
     </row>
-    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>107</v>
       </c>
       <c r="B204" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C204" t="s">
         <v>5</v>
       </c>
       <c r="E204" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F204" s="1">
         <v>44913</v>
@@ -9486,7 +9490,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>106</v>
       </c>
@@ -9497,7 +9501,7 @@
         <v>7</v>
       </c>
       <c r="E206" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F206" s="1">
         <v>44940</v>
@@ -9509,18 +9513,18 @@
         <v>218</v>
       </c>
     </row>
-    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>107</v>
       </c>
       <c r="B207" t="s">
+        <v>245</v>
+      </c>
+      <c r="C207" t="s">
+        <v>251</v>
+      </c>
+      <c r="E207" t="s">
         <v>246</v>
-      </c>
-      <c r="C207" t="s">
-        <v>252</v>
-      </c>
-      <c r="E207" t="s">
-        <v>247</v>
       </c>
       <c r="F207" s="1">
         <v>44946</v>
@@ -9535,18 +9539,18 @@
         <v>143</v>
       </c>
     </row>
-    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>107</v>
       </c>
       <c r="B208" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C208" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E208" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F208" s="1">
         <v>44946</v>
@@ -9561,7 +9565,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>103</v>
       </c>
@@ -9585,23 +9589,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I209" xr:uid="{8273E431-88A0-4D26-AA21-9E0D94FE2923}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Lameiro da ponte"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <customFilters and="1">
-        <customFilter operator="greaterThanOrEqual" val="44166"/>
-        <customFilter operator="lessThanOrEqual" val="45061"/>
-      </customFilters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I151">
-      <sortCondition ref="F2:F151"/>
-      <sortCondition ref="B2:B151"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:I209" xr:uid="{8273E431-88A0-4D26-AA21-9E0D94FE2923}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I209">
     <sortCondition ref="F2:F209"/>
     <sortCondition ref="A2:A209"/>

</xml_diff>